<commit_message>
Feat: Add Bristol Stool Chart (Phase 12)
</commit_message>
<xml_diff>
--- a/temp/pages/StructureDefinition-onc-goal-evaluation.xlsx
+++ b/temp/pages/StructureDefinition-onc-goal-evaluation.xlsx
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-12-26T14:13:58+00:00</t>
+    <t>2025-12-26T15:22:58+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -890,7 +890,7 @@
   </si>
   <si>
     <t>Quantity
-CodeableConcept</t>
+CodeableConceptstring</t>
   </si>
   <si>
     <t>Actual result</t>

</xml_diff>